<commit_message>
1. Cleaned up Correlation code. 2. Added Comprehensions examples 3. Added using closure for resources. 4. Added merge test.
</commit_message>
<xml_diff>
--- a/src/test/resources/Correlations.xlsx
+++ b/src/test/resources/Correlations.xlsx
@@ -293,7 +293,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="59">
+  <cellStyleXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -307,6 +307,9 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -449,6 +452,16 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="4" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="8" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="8" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="10" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="10" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -473,18 +486,8 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="4" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="4" xfId="4" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="8" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="8" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="6" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="6" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="10" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="10" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="4" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="59">
+  <cellStyles count="62">
     <cellStyle name="40% - Accent1" xfId="4" builtinId="31"/>
     <cellStyle name="40% - Accent2" xfId="6" builtinId="35"/>
     <cellStyle name="40% - Accent3" xfId="8" builtinId="39"/>
@@ -542,6 +545,9 @@
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -872,10 +878,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G560"/>
+  <dimension ref="A1:L560"/>
   <sheetViews>
-    <sheetView topLeftCell="A544" workbookViewId="0">
-      <selection activeCell="A549" sqref="A549"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -886,12 +892,12 @@
     <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:12">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -901,7 +907,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:12">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -923,8 +929,11 @@
       <c r="G3" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="2">
         <v>41556</v>
       </c>
@@ -940,8 +949,9 @@
       <c r="G4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="2">
         <v>41557</v>
       </c>
@@ -958,8 +968,9 @@
         <f>(B5-B4)/B4</f>
         <v>-2.513416208138065E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="2">
         <v>41558</v>
       </c>
@@ -976,8 +987,9 @@
         <f t="shared" ref="G6:G69" si="0">(B6-B5)/B5</f>
         <v>9.670389539634892E-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="2">
         <v>41559</v>
       </c>
@@ -994,8 +1006,9 @@
         <f t="shared" si="0"/>
         <v>5.7331714555512127E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="2">
         <v>41560</v>
       </c>
@@ -1012,8 +1025,9 @@
         <f t="shared" si="0"/>
         <v>2.4210314532895075E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="2">
         <v>41561</v>
       </c>
@@ -1030,8 +1044,9 @@
         <f t="shared" si="0"/>
         <v>4.7407019381875387E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="2">
         <v>41562</v>
       </c>
@@ -1048,8 +1063,9 @@
         <f t="shared" si="0"/>
         <v>-3.1507876969242433E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="2">
         <v>41563</v>
       </c>
@@ -1066,8 +1082,9 @@
         <f t="shared" si="0"/>
         <v>5.5189775367931911E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="2">
         <v>41564</v>
       </c>
@@ -1084,8 +1101,9 @@
         <f t="shared" si="0"/>
         <v>2.2939988988805286E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="2">
         <v>41565</v>
       </c>
@@ -1102,8 +1120,9 @@
         <f t="shared" si="0"/>
         <v>9.4665709843320248E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" s="2">
         <v>41566</v>
       </c>
@@ -1120,8 +1139,9 @@
         <f t="shared" si="0"/>
         <v>4.7090958754438542E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="2">
         <v>41567</v>
       </c>
@@ -1138,8 +1158,9 @@
         <f t="shared" si="0"/>
         <v>4.3303594720092483E-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="2">
         <v>41568</v>
       </c>
@@ -1156,8 +1177,9 @@
         <f t="shared" si="0"/>
         <v>8.4363636363636405E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="2">
         <v>41569</v>
       </c>
@@ -1174,8 +1196,9 @@
         <f t="shared" si="0"/>
         <v>6.9320686020887215E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="J17" s="4"/>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="2">
         <v>41570</v>
       </c>
@@ -1192,8 +1215,9 @@
         <f t="shared" si="0"/>
         <v>-4.9191344473813979E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="2">
         <v>41571</v>
       </c>
@@ -1210,8 +1234,9 @@
         <f t="shared" si="0"/>
         <v>-8.1609574518211353E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="J19" s="4"/>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="2">
         <v>41572</v>
       </c>
@@ -1228,8 +1253,9 @@
         <f t="shared" si="0"/>
         <v>6.8647067877481899E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="J20" s="4"/>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="2">
         <v>41573</v>
       </c>
@@ -1246,8 +1272,9 @@
         <f t="shared" si="0"/>
         <v>1.7283594987757427E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" s="2">
         <v>41575</v>
       </c>
@@ -1264,8 +1291,9 @@
         <f t="shared" si="0"/>
         <v>2.6098447307565255E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="J22" s="4"/>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="2">
         <v>41576</v>
       </c>
@@ -1282,8 +1310,9 @@
         <f t="shared" si="0"/>
         <v>1.5315978290865664E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" s="2">
         <v>41577</v>
       </c>
@@ -1301,7 +1330,7 @@
         <v>2.9671574178935498E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:10">
       <c r="A25" s="2">
         <v>41578</v>
       </c>
@@ -1319,7 +1348,7 @@
         <v>-4.4258688957325126E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:10">
       <c r="A26" s="2">
         <v>41579</v>
       </c>
@@ -1337,7 +1366,7 @@
         <v>4.2901859694347233E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:10">
       <c r="A27" s="2">
         <v>41580</v>
       </c>
@@ -1355,7 +1384,7 @@
         <v>-2.3128531073446368E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:10">
       <c r="A28" s="2">
         <v>41581</v>
       </c>
@@ -1373,7 +1402,7 @@
         <v>5.2864630399421728E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:10">
       <c r="A29" s="2">
         <v>41582</v>
       </c>
@@ -1391,7 +1420,7 @@
         <v>4.8708265384945472E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:10">
       <c r="A30" s="2">
         <v>41583</v>
       </c>
@@ -1409,7 +1438,7 @@
         <v>0.12792077587265208</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:10">
       <c r="A31" s="2">
         <v>41584</v>
       </c>
@@ -1427,7 +1456,7 @@
         <v>0.115916264557559</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:10">
       <c r="A32" s="2">
         <v>41585</v>
       </c>
@@ -13178,6 +13207,7 @@
     <hyperlink ref="B2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -13190,7 +13220,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C510"/>
   <sheetViews>
-    <sheetView topLeftCell="A502" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -19349,20 +19379,20 @@
       <c r="A1" s="25"/>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
-      <c r="D1" s="60" t="s">
+      <c r="D1" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="61"/>
-      <c r="F1" s="54" t="s">
+      <c r="E1" s="71"/>
+      <c r="F1" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="55"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="57" t="s">
+      <c r="G1" s="65"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="58"/>
-      <c r="K1" s="59"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="69"/>
       <c r="L1" s="27"/>
       <c r="M1" s="28"/>
       <c r="N1" s="29"/>
@@ -19465,8 +19495,8 @@
         <v>19</v>
       </c>
       <c r="R3">
-        <f>PEARSON(D3:D561,E3:E561)</f>
-        <v>7.3047279851036495E-4</v>
+        <f>PEARSON(D3:D572,E3:E572)</f>
+        <v>-4.706657597210501E-3</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -39450,7 +39480,7 @@
         <v>0</v>
       </c>
       <c r="D516" s="42">
-        <f t="shared" ref="D516:D579" si="62">IF(OR(ISNA(B516), ISNA(C516), B516=0, C516=0),0,B516)</f>
+        <f t="shared" ref="D516:D561" si="62">IF(OR(ISNA(B516), ISNA(C516), B516=0, C516=0),0,B516)</f>
         <v>0</v>
       </c>
       <c r="E516" s="40">
@@ -41193,14 +41223,14 @@
       <c r="N560" s="12"/>
     </row>
     <row r="561" spans="1:14">
-      <c r="A561" s="62">
+      <c r="A561" s="54">
         <v>42114</v>
       </c>
       <c r="B561" s="32">
         <f t="shared" si="56"/>
         <v>-3.1526336024606021E-2</v>
       </c>
-      <c r="C561" s="70">
+      <c r="C561" s="62">
         <f t="shared" si="57"/>
         <v>-6.4791133844842282E-3</v>
       </c>
@@ -41232,14 +41262,14 @@
       <c r="N561" s="12"/>
     </row>
     <row r="562" spans="1:14">
-      <c r="A562" s="62">
+      <c r="A562" s="54">
         <v>42115</v>
       </c>
       <c r="B562" s="32">
         <f t="shared" si="56"/>
         <v>1.0123064708217555E-2</v>
       </c>
-      <c r="C562" s="70">
+      <c r="C562" s="62">
         <f t="shared" ref="C562:C572" si="63">IF(ISNA(VLOOKUP(A562,asx_spi200_with_returns, 3, FALSE)),0,VLOOKUP(A562,asx_spi200_with_returns, 3, FALSE))</f>
         <v>8.58074480864939E-3</v>
       </c>
@@ -41247,7 +41277,7 @@
         <f t="shared" ref="D562:D572" si="64">IF(OR(ISNA(B562), ISNA(C562), B562=0, C562=0),0,B562)</f>
         <v>1.0123064708217555E-2</v>
       </c>
-      <c r="E562" s="68">
+      <c r="E562" s="60">
         <f t="shared" ref="E562:E572" si="65">IF(OR(B562=0, C562=0),0,C562)</f>
         <v>8.58074480864939E-3</v>
       </c>
@@ -41256,13 +41286,13 @@
         <f t="shared" ref="G562:G572" si="66">(D562-$F$3)^2</f>
         <v>1.0056315186691973E-4</v>
       </c>
-      <c r="H562" s="66"/>
+      <c r="H562" s="58"/>
       <c r="I562" s="18"/>
       <c r="J562" s="18">
         <f t="shared" ref="J562:J572" si="67">(E562-$I$3)^2</f>
         <v>6.9527352449851124E-5</v>
       </c>
-      <c r="K562" s="64"/>
+      <c r="K562" s="56"/>
       <c r="L562" s="11">
         <f t="shared" ref="L562:L572" si="68">(D562-$F$3)*(E562-$I$3)</f>
         <v>8.3617520313145091E-5</v>
@@ -41271,14 +41301,14 @@
       <c r="N562" s="12"/>
     </row>
     <row r="563" spans="1:14">
-      <c r="A563" s="62">
+      <c r="A563" s="54">
         <v>42116</v>
       </c>
       <c r="B563" s="32">
         <f t="shared" si="56"/>
         <v>2.5348791511102409E-2</v>
       </c>
-      <c r="C563" s="70">
+      <c r="C563" s="62">
         <f t="shared" si="63"/>
         <v>-9.0182065679768591E-3</v>
       </c>
@@ -41286,7 +41316,7 @@
         <f t="shared" si="64"/>
         <v>2.5348791511102409E-2</v>
       </c>
-      <c r="E563" s="68">
+      <c r="E563" s="60">
         <f t="shared" si="65"/>
         <v>-9.0182065679768591E-3</v>
       </c>
@@ -41295,13 +41325,13 @@
         <f t="shared" si="66"/>
         <v>6.3775668046347144E-4</v>
       </c>
-      <c r="H563" s="66"/>
+      <c r="H563" s="58"/>
       <c r="I563" s="18"/>
       <c r="J563" s="18">
         <f t="shared" si="67"/>
         <v>8.5759546683009479E-5</v>
       </c>
-      <c r="K563" s="64"/>
+      <c r="K563" s="56"/>
       <c r="L563" s="11">
         <f t="shared" si="68"/>
         <v>-2.3386689336160483E-4</v>
@@ -41310,14 +41340,14 @@
       <c r="N563" s="12"/>
     </row>
     <row r="564" spans="1:14">
-      <c r="A564" s="62">
+      <c r="A564" s="54">
         <v>42117</v>
       </c>
       <c r="B564" s="32">
         <f t="shared" si="56"/>
         <v>1.1115369873514816E-2</v>
       </c>
-      <c r="C564" s="70">
+      <c r="C564" s="62">
         <f t="shared" si="63"/>
         <v>1.201923076923077E-3</v>
       </c>
@@ -41325,7 +41355,7 @@
         <f t="shared" si="64"/>
         <v>1.1115369873514816E-2</v>
       </c>
-      <c r="E564" s="68">
+      <c r="E564" s="60">
         <f t="shared" si="65"/>
         <v>1.201923076923077E-3</v>
       </c>
@@ -41334,13 +41364,13 @@
         <f t="shared" si="66"/>
         <v>1.214497281104114E-4</v>
       </c>
-      <c r="H564" s="66"/>
+      <c r="H564" s="58"/>
       <c r="I564" s="18"/>
       <c r="J564" s="18">
         <f t="shared" si="67"/>
         <v>9.2061069397150598E-7</v>
       </c>
-      <c r="K564" s="64"/>
+      <c r="K564" s="56"/>
       <c r="L564" s="11">
         <f t="shared" si="68"/>
         <v>1.0573926351094779E-5</v>
@@ -41349,14 +41379,14 @@
       <c r="N564" s="12"/>
     </row>
     <row r="565" spans="1:14">
-      <c r="A565" s="62">
+      <c r="A565" s="54">
         <v>42118</v>
       </c>
       <c r="B565" s="32">
         <f t="shared" si="56"/>
         <v>-3.0673490017690104E-2</v>
       </c>
-      <c r="C565" s="70">
+      <c r="C565" s="62">
         <f t="shared" si="63"/>
         <v>1.8350197221745843E-2</v>
       </c>
@@ -41364,7 +41394,7 @@
         <f t="shared" si="64"/>
         <v>-3.0673490017690104E-2</v>
       </c>
-      <c r="E565" s="68">
+      <c r="E565" s="60">
         <f t="shared" si="65"/>
         <v>1.8350197221745843E-2</v>
       </c>
@@ -41373,13 +41403,13 @@
         <f t="shared" si="66"/>
         <v>9.466966947362668E-4</v>
       </c>
-      <c r="H565" s="66"/>
+      <c r="H565" s="58"/>
       <c r="I565" s="18"/>
       <c r="J565" s="18">
         <f t="shared" si="67"/>
         <v>3.2789092669152571E-4</v>
       </c>
-      <c r="K565" s="64"/>
+      <c r="K565" s="56"/>
       <c r="L565" s="11">
         <f t="shared" si="68"/>
         <v>-5.5714742800526233E-4</v>
@@ -41388,14 +41418,14 @@
       <c r="N565" s="12"/>
     </row>
     <row r="566" spans="1:14">
-      <c r="A566" s="62">
+      <c r="A566" s="54">
         <v>42119</v>
       </c>
       <c r="B566" s="32">
         <f t="shared" si="56"/>
         <v>-5.1490956493402016E-3</v>
       </c>
-      <c r="C566" s="70">
+      <c r="C566" s="62">
         <f t="shared" si="63"/>
         <v>0</v>
       </c>
@@ -41403,7 +41433,7 @@
         <f t="shared" si="64"/>
         <v>0</v>
       </c>
-      <c r="E566" s="68">
+      <c r="E566" s="60">
         <f t="shared" si="65"/>
         <v>0</v>
       </c>
@@ -41412,13 +41442,13 @@
         <f t="shared" si="66"/>
         <v>9.0148656136734644E-9</v>
       </c>
-      <c r="H566" s="66"/>
+      <c r="H566" s="58"/>
       <c r="I566" s="18"/>
       <c r="J566" s="18">
         <f t="shared" si="67"/>
         <v>5.8776416019003168E-8</v>
       </c>
-      <c r="K566" s="64"/>
+      <c r="K566" s="56"/>
       <c r="L566" s="11">
         <f t="shared" si="68"/>
         <v>2.3018720461065549E-8</v>
@@ -41427,14 +41457,14 @@
       <c r="N566" s="12"/>
     </row>
     <row r="567" spans="1:14">
-      <c r="A567" s="62">
+      <c r="A567" s="54">
         <v>42120</v>
       </c>
       <c r="B567" s="32">
         <f t="shared" si="56"/>
         <v>7.0429455891507006E-3</v>
       </c>
-      <c r="C567" s="70">
+      <c r="C567" s="62">
         <f t="shared" si="63"/>
         <v>0</v>
       </c>
@@ -41442,7 +41472,7 @@
         <f t="shared" si="64"/>
         <v>0</v>
       </c>
-      <c r="E567" s="68">
+      <c r="E567" s="60">
         <f t="shared" si="65"/>
         <v>0</v>
       </c>
@@ -41451,13 +41481,13 @@
         <f t="shared" si="66"/>
         <v>9.0148656136734644E-9</v>
       </c>
-      <c r="H567" s="66"/>
+      <c r="H567" s="58"/>
       <c r="I567" s="18"/>
       <c r="J567" s="18">
         <f t="shared" si="67"/>
         <v>5.8776416019003168E-8</v>
       </c>
-      <c r="K567" s="64"/>
+      <c r="K567" s="56"/>
       <c r="L567" s="11">
         <f t="shared" si="68"/>
         <v>2.3018720461065549E-8</v>
@@ -41466,14 +41496,14 @@
       <c r="N567" s="12"/>
     </row>
     <row r="568" spans="1:14">
-      <c r="A568" s="62">
+      <c r="A568" s="54">
         <v>42121</v>
       </c>
       <c r="B568" s="32">
         <f t="shared" si="56"/>
         <v>-4.0010409212152792E-2</v>
       </c>
-      <c r="C568" s="70">
+      <c r="C568" s="62">
         <f t="shared" si="63"/>
         <v>5.7258336140114515E-3</v>
       </c>
@@ -41481,7 +41511,7 @@
         <f t="shared" si="64"/>
         <v>-4.0010409212152792E-2</v>
       </c>
-      <c r="E568" s="68">
+      <c r="E568" s="60">
         <f t="shared" si="65"/>
         <v>5.7258336140114515E-3</v>
       </c>
@@ -41490,13 +41520,13 @@
         <f t="shared" si="66"/>
         <v>1.6084395685204854E-3</v>
       </c>
-      <c r="H568" s="66"/>
+      <c r="H568" s="58"/>
       <c r="I568" s="18"/>
       <c r="J568" s="18">
         <f t="shared" si="67"/>
         <v>3.0067622208495452E-5</v>
       </c>
-      <c r="K568" s="64"/>
+      <c r="K568" s="56"/>
       <c r="L568" s="11">
         <f t="shared" si="68"/>
         <v>-2.1991351320796407E-4</v>
@@ -41505,14 +41535,14 @@
       <c r="N568" s="12"/>
     </row>
     <row r="569" spans="1:14">
-      <c r="A569" s="62">
+      <c r="A569" s="54">
         <v>42122</v>
       </c>
       <c r="B569" s="32">
         <f t="shared" si="56"/>
         <v>-3.5917592843589126E-3</v>
       </c>
-      <c r="C569" s="70">
+      <c r="C569" s="62">
         <f t="shared" si="63"/>
         <v>-7.7026121902210318E-3</v>
       </c>
@@ -41520,7 +41550,7 @@
         <f t="shared" si="64"/>
         <v>-3.5917592843589126E-3</v>
       </c>
-      <c r="E569" s="68">
+      <c r="E569" s="60">
         <f t="shared" si="65"/>
         <v>-7.7026121902210318E-3</v>
       </c>
@@ -41529,13 +41559,13 @@
         <f t="shared" si="66"/>
         <v>1.3591800617992903E-5</v>
       </c>
-      <c r="H569" s="66"/>
+      <c r="H569" s="58"/>
       <c r="I569" s="18"/>
       <c r="J569" s="18">
         <f t="shared" si="67"/>
         <v>6.3123830133840654E-5</v>
       </c>
-      <c r="K569" s="64"/>
+      <c r="K569" s="56"/>
       <c r="L569" s="11">
         <f t="shared" si="68"/>
         <v>2.9291065419735321E-5</v>
@@ -41544,14 +41574,14 @@
       <c r="N569" s="12"/>
     </row>
     <row r="570" spans="1:14">
-      <c r="A570" s="62">
+      <c r="A570" s="54">
         <v>42123</v>
       </c>
       <c r="B570" s="32">
         <f t="shared" si="56"/>
         <v>2.1356185812419142E-2</v>
       </c>
-      <c r="C570" s="70">
+      <c r="C570" s="62">
         <f t="shared" si="63"/>
         <v>-1.670604117448532E-2</v>
       </c>
@@ -41559,7 +41589,7 @@
         <f t="shared" si="64"/>
         <v>2.1356185812419142E-2</v>
       </c>
-      <c r="E570" s="68">
+      <c r="E570" s="60">
         <f t="shared" si="65"/>
         <v>-1.670604117448532E-2</v>
       </c>
@@ -41568,13 +41598,13 @@
         <f t="shared" si="66"/>
         <v>4.5204029088562387E-4</v>
       </c>
-      <c r="H570" s="66"/>
+      <c r="H570" s="58"/>
       <c r="I570" s="18"/>
       <c r="J570" s="18">
         <f t="shared" si="67"/>
         <v>2.8725096255895514E-4</v>
       </c>
-      <c r="K570" s="64"/>
+      <c r="K570" s="56"/>
       <c r="L570" s="11">
         <f t="shared" si="68"/>
         <v>-3.6034567941398371E-4</v>
@@ -41583,14 +41613,14 @@
       <c r="N570" s="12"/>
     </row>
     <row r="571" spans="1:14">
-      <c r="A571" s="62">
+      <c r="A571" s="54">
         <v>42124</v>
       </c>
       <c r="B571" s="32">
         <f t="shared" si="56"/>
         <v>-1.3984151295198737E-2</v>
       </c>
-      <c r="C571" s="70">
+      <c r="C571" s="62">
         <f t="shared" si="63"/>
         <v>-1.2013042732109147E-2</v>
       </c>
@@ -41598,7 +41628,7 @@
         <f t="shared" si="64"/>
         <v>-1.3984151295198737E-2</v>
       </c>
-      <c r="E571" s="68">
+      <c r="E571" s="60">
         <f t="shared" si="65"/>
         <v>-1.2013042732109147E-2</v>
       </c>
@@ -41607,13 +41637,13 @@
         <f t="shared" si="66"/>
         <v>1.9822099884187378E-4</v>
       </c>
-      <c r="H571" s="66"/>
+      <c r="H571" s="58"/>
       <c r="I571" s="18"/>
       <c r="J571" s="18">
         <f t="shared" si="67"/>
         <v>1.5019681971176329E-4</v>
       </c>
-      <c r="K571" s="64"/>
+      <c r="K571" s="56"/>
       <c r="L571" s="11">
         <f t="shared" si="68"/>
         <v>1.7254612028712367E-4</v>
@@ -41622,14 +41652,14 @@
       <c r="N571" s="12"/>
     </row>
     <row r="572" spans="1:14">
-      <c r="A572" s="63">
+      <c r="A572" s="55">
         <v>42125</v>
       </c>
       <c r="B572" s="36">
         <f t="shared" si="56"/>
         <v>3.231579658269735E-2</v>
       </c>
-      <c r="C572" s="71">
+      <c r="C572" s="63">
         <f t="shared" si="63"/>
         <v>7.2954663887441372E-3</v>
       </c>
@@ -41637,7 +41667,7 @@
         <f t="shared" si="64"/>
         <v>3.231579658269735E-2</v>
       </c>
-      <c r="E572" s="69">
+      <c r="E572" s="61">
         <f t="shared" si="65"/>
         <v>7.2954663887441372E-3</v>
       </c>
@@ -41646,13 +41676,13 @@
         <f t="shared" si="66"/>
         <v>1.0381831706339987E-3</v>
       </c>
-      <c r="H572" s="67"/>
+      <c r="H572" s="59"/>
       <c r="I572" s="19"/>
       <c r="J572" s="19">
         <f t="shared" si="67"/>
         <v>4.9745202697981276E-5</v>
       </c>
-      <c r="K572" s="65"/>
+      <c r="K572" s="57"/>
       <c r="L572" s="13">
         <f t="shared" si="68"/>
         <v>2.2725455388357161E-4</v>

</xml_diff>